<commit_message>
Blocklisted word changes [MOSIP-28207]
Signed-off-by: GOKULRAJ136 <110164849+GOKULRAJ136@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/blocklisted_words.xlsx
+++ b/mosip_master/xlsx/blocklisted_words.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gokulraj\Documents\GitHub\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D287EB-930C-42A9-BDD7-F24F519C0755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9628C418-2204-4629-931A-AD15AC08E158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>shit</t>
   </si>
   <si>
-    <t>Blacklisted Word</t>
-  </si>
-  <si>
     <t>TRUE</t>
   </si>
   <si>
@@ -66,10 +63,13 @@
     <t>Merde</t>
   </si>
   <si>
-    <t>Mot sur la liste noire</t>
-  </si>
-  <si>
     <t>bon sang</t>
+  </si>
+  <si>
+    <t>Mot sur la liste de blocage</t>
+  </si>
+  <si>
+    <t>Blocklisted Word</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -516,13 +516,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -530,13 +530,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -544,41 +544,41 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>